<commit_message>
adjust to work for both cases
</commit_message>
<xml_diff>
--- a/src/last_fm_output.xlsx
+++ b/src/last_fm_output.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sicon\Documents\GitHub\Law-School-Copyright\src\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62653C6A-7E46-4494-A982-2DFF744C974D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="1963" sheetId="1" r:id="rId1"/>
     <sheet name="1964" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -1304,8 +1298,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1368,14 +1362,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1422,7 +1408,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1454,27 +1440,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1506,24 +1474,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1699,20 +1649,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1729,7 +1673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1740,16 +1684,16 @@
         <v>92</v>
       </c>
       <c r="D2">
-        <v>861009</v>
+        <v>861127</v>
       </c>
       <c r="E2">
-        <v>239577</v>
+        <v>239614</v>
       </c>
       <c r="F2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1760,16 +1704,16 @@
         <v>93</v>
       </c>
       <c r="D3">
-        <v>847156</v>
+        <v>847994</v>
       </c>
       <c r="E3">
-        <v>163657</v>
+        <v>163769</v>
       </c>
       <c r="F3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1780,16 +1724,16 @@
         <v>94</v>
       </c>
       <c r="D4">
-        <v>212262</v>
+        <v>212415</v>
       </c>
       <c r="E4">
-        <v>51147</v>
+        <v>51183</v>
       </c>
       <c r="F4" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1800,16 +1744,16 @@
         <v>95</v>
       </c>
       <c r="D5">
-        <v>309177</v>
+        <v>309215</v>
       </c>
       <c r="E5">
-        <v>92437</v>
+        <v>92444</v>
       </c>
       <c r="F5" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1820,16 +1764,16 @@
         <v>96</v>
       </c>
       <c r="D6">
-        <v>593927</v>
+        <v>594537</v>
       </c>
       <c r="E6">
-        <v>143773</v>
+        <v>143897</v>
       </c>
       <c r="F6" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1840,16 +1784,16 @@
         <v>97</v>
       </c>
       <c r="D7">
-        <v>107544</v>
+        <v>107573</v>
       </c>
       <c r="E7">
-        <v>32417</v>
+        <v>32425</v>
       </c>
       <c r="F7" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1860,7 +1804,7 @@
         <v>98</v>
       </c>
       <c r="D8">
-        <v>50819</v>
+        <v>50836</v>
       </c>
       <c r="E8">
         <v>24329</v>
@@ -1869,7 +1813,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1880,16 +1824,16 @@
         <v>99</v>
       </c>
       <c r="D9">
-        <v>135085</v>
+        <v>135126</v>
       </c>
       <c r="E9">
-        <v>48471</v>
+        <v>48483</v>
       </c>
       <c r="F9" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1900,16 +1844,16 @@
         <v>100</v>
       </c>
       <c r="D10">
-        <v>178277</v>
+        <v>178337</v>
       </c>
       <c r="E10">
-        <v>53422</v>
+        <v>53445</v>
       </c>
       <c r="F10" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1920,16 +1864,16 @@
         <v>101</v>
       </c>
       <c r="D11">
-        <v>189263</v>
+        <v>189607</v>
       </c>
       <c r="E11">
-        <v>40594</v>
+        <v>40620</v>
       </c>
       <c r="F11" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1940,16 +1884,16 @@
         <v>102</v>
       </c>
       <c r="D12">
-        <v>47880</v>
+        <v>47898</v>
       </c>
       <c r="E12">
-        <v>16028</v>
+        <v>16036</v>
       </c>
       <c r="F12" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1960,16 +1904,16 @@
         <v>103</v>
       </c>
       <c r="D13">
-        <v>135569</v>
+        <v>135658</v>
       </c>
       <c r="E13">
-        <v>31022</v>
+        <v>31042</v>
       </c>
       <c r="F13" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1980,16 +1924,16 @@
         <v>104</v>
       </c>
       <c r="D14">
-        <v>110503</v>
+        <v>110567</v>
       </c>
       <c r="E14">
-        <v>26313</v>
+        <v>26334</v>
       </c>
       <c r="F14" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2000,16 +1944,16 @@
         <v>105</v>
       </c>
       <c r="D15">
-        <v>333235</v>
+        <v>333367</v>
       </c>
       <c r="E15">
-        <v>104036</v>
+        <v>104072</v>
       </c>
       <c r="F15" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2020,16 +1964,16 @@
         <v>106</v>
       </c>
       <c r="D16">
-        <v>30461</v>
+        <v>30464</v>
       </c>
       <c r="E16">
-        <v>14348</v>
+        <v>14349</v>
       </c>
       <c r="F16" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2049,7 +1993,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2060,7 +2004,7 @@
         <v>108</v>
       </c>
       <c r="D18">
-        <v>22663</v>
+        <v>22665</v>
       </c>
       <c r="E18">
         <v>10292</v>
@@ -2069,7 +2013,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2080,16 +2024,16 @@
         <v>109</v>
       </c>
       <c r="D19">
-        <v>56891</v>
+        <v>56897</v>
       </c>
       <c r="E19">
-        <v>17255</v>
+        <v>17258</v>
       </c>
       <c r="F19" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2100,7 +2044,7 @@
         <v>110</v>
       </c>
       <c r="D20">
-        <v>14658</v>
+        <v>14661</v>
       </c>
       <c r="E20">
         <v>5712</v>
@@ -2109,7 +2053,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2120,16 +2064,16 @@
         <v>111</v>
       </c>
       <c r="D21">
-        <v>148795</v>
+        <v>148876</v>
       </c>
       <c r="E21">
-        <v>34236</v>
+        <v>34255</v>
       </c>
       <c r="F21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2140,16 +2084,16 @@
         <v>112</v>
       </c>
       <c r="D22">
-        <v>197494</v>
+        <v>197548</v>
       </c>
       <c r="E22">
-        <v>58672</v>
+        <v>58691</v>
       </c>
       <c r="F22" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2160,16 +2104,16 @@
         <v>113</v>
       </c>
       <c r="D23">
-        <v>221422</v>
+        <v>221475</v>
       </c>
       <c r="E23">
-        <v>82142</v>
+        <v>82157</v>
       </c>
       <c r="F23" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2180,16 +2124,16 @@
         <v>114</v>
       </c>
       <c r="D24">
-        <v>570816</v>
+        <v>571095</v>
       </c>
       <c r="E24">
-        <v>145424</v>
+        <v>145495</v>
       </c>
       <c r="F24" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2200,16 +2144,16 @@
         <v>115</v>
       </c>
       <c r="D25">
-        <v>10478</v>
+        <v>10492</v>
       </c>
       <c r="E25">
-        <v>2698</v>
+        <v>2701</v>
       </c>
       <c r="F25" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2220,7 +2164,7 @@
         <v>116</v>
       </c>
       <c r="D26">
-        <v>17261</v>
+        <v>17266</v>
       </c>
       <c r="E26">
         <v>6798</v>
@@ -2229,7 +2173,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2240,7 +2184,7 @@
         <v>117</v>
       </c>
       <c r="D27">
-        <v>61748</v>
+        <v>61754</v>
       </c>
       <c r="E27">
         <v>18358</v>
@@ -2249,7 +2193,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2260,16 +2204,16 @@
         <v>118</v>
       </c>
       <c r="D28">
-        <v>96497</v>
+        <v>96526</v>
       </c>
       <c r="E28">
-        <v>26454</v>
+        <v>26462</v>
       </c>
       <c r="F28" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2280,16 +2224,16 @@
         <v>119</v>
       </c>
       <c r="D29">
-        <v>157532</v>
+        <v>157559</v>
       </c>
       <c r="E29">
-        <v>51769</v>
+        <v>51779</v>
       </c>
       <c r="F29" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2300,16 +2244,16 @@
         <v>120</v>
       </c>
       <c r="D30">
-        <v>197962</v>
+        <v>198007</v>
       </c>
       <c r="E30">
-        <v>44512</v>
+        <v>44521</v>
       </c>
       <c r="F30" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2320,16 +2264,16 @@
         <v>121</v>
       </c>
       <c r="D31">
-        <v>128341</v>
+        <v>128360</v>
       </c>
       <c r="E31">
-        <v>37850</v>
+        <v>37853</v>
       </c>
       <c r="F31" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2340,7 +2284,7 @@
         <v>122</v>
       </c>
       <c r="D32">
-        <v>33188</v>
+        <v>33190</v>
       </c>
       <c r="E32">
         <v>9171</v>
@@ -2349,7 +2293,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2360,16 +2304,16 @@
         <v>123</v>
       </c>
       <c r="D33">
-        <v>43739</v>
+        <v>43758</v>
       </c>
       <c r="E33">
-        <v>18117</v>
+        <v>18125</v>
       </c>
       <c r="F33" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2380,16 +2324,16 @@
         <v>124</v>
       </c>
       <c r="D34">
-        <v>32575</v>
+        <v>32577</v>
       </c>
       <c r="E34">
-        <v>9677</v>
+        <v>9678</v>
       </c>
       <c r="F34" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2400,16 +2344,16 @@
         <v>125</v>
       </c>
       <c r="D35">
-        <v>179804</v>
+        <v>180070</v>
       </c>
       <c r="E35">
-        <v>43646</v>
+        <v>43680</v>
       </c>
       <c r="F35" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2420,16 +2364,16 @@
         <v>126</v>
       </c>
       <c r="D36">
-        <v>2175424</v>
+        <v>2176767</v>
       </c>
       <c r="E36">
-        <v>443492</v>
+        <v>443722</v>
       </c>
       <c r="F36" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2440,16 +2384,16 @@
         <v>127</v>
       </c>
       <c r="D37">
-        <v>17043</v>
+        <v>17045</v>
       </c>
       <c r="E37">
-        <v>6678</v>
+        <v>6680</v>
       </c>
       <c r="F37" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2460,16 +2404,16 @@
         <v>128</v>
       </c>
       <c r="D38">
-        <v>44185</v>
+        <v>44194</v>
       </c>
       <c r="E38">
-        <v>14199</v>
+        <v>14204</v>
       </c>
       <c r="F38" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2480,16 +2424,16 @@
         <v>129</v>
       </c>
       <c r="D39">
-        <v>46050</v>
+        <v>46061</v>
       </c>
       <c r="E39">
-        <v>16968</v>
+        <v>16971</v>
       </c>
       <c r="F39" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2500,16 +2444,16 @@
         <v>130</v>
       </c>
       <c r="D40">
-        <v>7615</v>
+        <v>7616</v>
       </c>
       <c r="E40">
-        <v>2321</v>
+        <v>2322</v>
       </c>
       <c r="F40" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2529,7 +2473,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2549,7 +2493,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2560,16 +2504,16 @@
         <v>133</v>
       </c>
       <c r="D43">
-        <v>95322</v>
+        <v>95355</v>
       </c>
       <c r="E43">
-        <v>31563</v>
+        <v>31566</v>
       </c>
       <c r="F43" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2589,7 +2533,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2600,16 +2544,16 @@
         <v>135</v>
       </c>
       <c r="D45">
-        <v>35166</v>
+        <v>35172</v>
       </c>
       <c r="E45">
-        <v>12471</v>
+        <v>12473</v>
       </c>
       <c r="F45" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2620,16 +2564,16 @@
         <v>136</v>
       </c>
       <c r="D46">
-        <v>239725</v>
+        <v>239735</v>
       </c>
       <c r="E46">
-        <v>84550</v>
+        <v>84551</v>
       </c>
       <c r="F46" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2640,16 +2584,16 @@
         <v>137</v>
       </c>
       <c r="D47">
-        <v>245479</v>
+        <v>245556</v>
       </c>
       <c r="E47">
-        <v>71529</v>
+        <v>71542</v>
       </c>
       <c r="F47" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2660,16 +2604,16 @@
         <v>138</v>
       </c>
       <c r="D48">
-        <v>57393</v>
+        <v>57402</v>
       </c>
       <c r="E48">
-        <v>22229</v>
+        <v>22233</v>
       </c>
       <c r="F48" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2680,16 +2624,16 @@
         <v>139</v>
       </c>
       <c r="D49">
-        <v>23548</v>
+        <v>23553</v>
       </c>
       <c r="E49">
-        <v>8928</v>
+        <v>8932</v>
       </c>
       <c r="F49" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2700,16 +2644,16 @@
         <v>140</v>
       </c>
       <c r="D50">
-        <v>924638</v>
+        <v>925191</v>
       </c>
       <c r="E50">
-        <v>208655</v>
+        <v>208741</v>
       </c>
       <c r="F50" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2729,7 +2673,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2740,16 +2684,16 @@
         <v>142</v>
       </c>
       <c r="D52">
-        <v>49903</v>
+        <v>49928</v>
       </c>
       <c r="E52">
-        <v>14072</v>
+        <v>14076</v>
       </c>
       <c r="F52" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2760,16 +2704,16 @@
         <v>143</v>
       </c>
       <c r="D53">
-        <v>30653</v>
+        <v>30669</v>
       </c>
       <c r="E53">
-        <v>8307</v>
+        <v>8317</v>
       </c>
       <c r="F53" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2780,16 +2724,16 @@
         <v>144</v>
       </c>
       <c r="D54">
-        <v>147613</v>
+        <v>147637</v>
       </c>
       <c r="E54">
-        <v>53063</v>
+        <v>53066</v>
       </c>
       <c r="F54" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2800,7 +2744,7 @@
         <v>145</v>
       </c>
       <c r="D55">
-        <v>17163</v>
+        <v>17164</v>
       </c>
       <c r="E55">
         <v>5427</v>
@@ -2809,7 +2753,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2820,16 +2764,16 @@
         <v>146</v>
       </c>
       <c r="D56">
-        <v>168146</v>
+        <v>168173</v>
       </c>
       <c r="E56">
-        <v>76281</v>
+        <v>76282</v>
       </c>
       <c r="F56" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2840,16 +2784,16 @@
         <v>147</v>
       </c>
       <c r="D57">
-        <v>249645</v>
+        <v>249770</v>
       </c>
       <c r="E57">
-        <v>89575</v>
+        <v>89611</v>
       </c>
       <c r="F57" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2860,16 +2804,16 @@
         <v>148</v>
       </c>
       <c r="D58">
-        <v>51566</v>
+        <v>51587</v>
       </c>
       <c r="E58">
-        <v>18129</v>
+        <v>18136</v>
       </c>
       <c r="F58" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2880,16 +2824,16 @@
         <v>149</v>
       </c>
       <c r="D59">
-        <v>758565</v>
+        <v>759047</v>
       </c>
       <c r="E59">
-        <v>181160</v>
+        <v>181260</v>
       </c>
       <c r="F59" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2900,16 +2844,16 @@
         <v>150</v>
       </c>
       <c r="D60">
-        <v>25764</v>
+        <v>25773</v>
       </c>
       <c r="E60">
-        <v>8705</v>
+        <v>8706</v>
       </c>
       <c r="F60" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2920,16 +2864,16 @@
         <v>151</v>
       </c>
       <c r="D61">
-        <v>36878</v>
+        <v>36894</v>
       </c>
       <c r="E61">
-        <v>11642</v>
+        <v>11647</v>
       </c>
       <c r="F61" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2940,16 +2884,16 @@
         <v>152</v>
       </c>
       <c r="D62">
-        <v>129733</v>
+        <v>129759</v>
       </c>
       <c r="E62">
-        <v>44619</v>
+        <v>44626</v>
       </c>
       <c r="F62" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2960,16 +2904,16 @@
         <v>153</v>
       </c>
       <c r="D63">
-        <v>37129</v>
+        <v>37140</v>
       </c>
       <c r="E63">
-        <v>12326</v>
+        <v>12328</v>
       </c>
       <c r="F63" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2980,16 +2924,16 @@
         <v>154</v>
       </c>
       <c r="D64">
-        <v>41863</v>
+        <v>41882</v>
       </c>
       <c r="E64">
-        <v>13214</v>
+        <v>13219</v>
       </c>
       <c r="F64" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -3000,16 +2944,16 @@
         <v>155</v>
       </c>
       <c r="D65">
-        <v>322980</v>
+        <v>323086</v>
       </c>
       <c r="E65">
-        <v>103523</v>
+        <v>103555</v>
       </c>
       <c r="F65" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -3029,7 +2973,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -3040,7 +2984,7 @@
         <v>157</v>
       </c>
       <c r="D67">
-        <v>33031</v>
+        <v>33032</v>
       </c>
       <c r="E67">
         <v>11683</v>
@@ -3049,7 +2993,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -3060,16 +3004,16 @@
         <v>158</v>
       </c>
       <c r="D68">
-        <v>144664</v>
+        <v>144710</v>
       </c>
       <c r="E68">
-        <v>52906</v>
+        <v>52918</v>
       </c>
       <c r="F68" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -3080,16 +3024,16 @@
         <v>159</v>
       </c>
       <c r="D69">
-        <v>14526</v>
+        <v>14532</v>
       </c>
       <c r="E69">
-        <v>4616</v>
+        <v>4618</v>
       </c>
       <c r="F69" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -3100,16 +3044,16 @@
         <v>160</v>
       </c>
       <c r="D70">
-        <v>3976466</v>
+        <v>3977561</v>
       </c>
       <c r="E70">
-        <v>783129</v>
+        <v>783284</v>
       </c>
       <c r="F70" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -3120,16 +3064,16 @@
         <v>161</v>
       </c>
       <c r="D71">
-        <v>170803</v>
+        <v>170897</v>
       </c>
       <c r="E71">
-        <v>46817</v>
+        <v>46843</v>
       </c>
       <c r="F71" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -3149,7 +3093,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -3160,16 +3104,16 @@
         <v>163</v>
       </c>
       <c r="D73">
-        <v>69890</v>
+        <v>69925</v>
       </c>
       <c r="E73">
-        <v>22796</v>
+        <v>22807</v>
       </c>
       <c r="F73" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -3180,16 +3124,16 @@
         <v>164</v>
       </c>
       <c r="D74">
-        <v>10072</v>
+        <v>10074</v>
       </c>
       <c r="E74">
-        <v>2985</v>
+        <v>2986</v>
       </c>
       <c r="F74" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -3209,7 +3153,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -3220,16 +3164,16 @@
         <v>166</v>
       </c>
       <c r="D76">
-        <v>23148</v>
+        <v>23254</v>
       </c>
       <c r="E76">
-        <v>6334</v>
+        <v>6372</v>
       </c>
       <c r="F76" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -3240,16 +3184,16 @@
         <v>167</v>
       </c>
       <c r="D77">
-        <v>42612</v>
+        <v>42628</v>
       </c>
       <c r="E77">
-        <v>15557</v>
+        <v>15558</v>
       </c>
       <c r="F77" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -3260,7 +3204,7 @@
         <v>168</v>
       </c>
       <c r="D78">
-        <v>25942</v>
+        <v>25946</v>
       </c>
       <c r="E78">
         <v>9227</v>
@@ -3269,7 +3213,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -3280,16 +3224,16 @@
         <v>169</v>
       </c>
       <c r="D79">
-        <v>348812</v>
+        <v>348956</v>
       </c>
       <c r="E79">
-        <v>95240</v>
+        <v>95276</v>
       </c>
       <c r="F79" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -3300,16 +3244,16 @@
         <v>170</v>
       </c>
       <c r="D80">
-        <v>9328</v>
+        <v>9329</v>
       </c>
       <c r="E80">
-        <v>5652</v>
+        <v>5653</v>
       </c>
       <c r="F80" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -3320,16 +3264,16 @@
         <v>171</v>
       </c>
       <c r="D81">
-        <v>15424</v>
+        <v>15431</v>
       </c>
       <c r="E81">
-        <v>5132</v>
+        <v>5134</v>
       </c>
       <c r="F81" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -3340,16 +3284,16 @@
         <v>172</v>
       </c>
       <c r="D82">
-        <v>87554</v>
+        <v>87572</v>
       </c>
       <c r="E82">
-        <v>32779</v>
+        <v>32790</v>
       </c>
       <c r="F82" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -3360,7 +3304,7 @@
         <v>173</v>
       </c>
       <c r="D83">
-        <v>3477</v>
+        <v>3479</v>
       </c>
       <c r="E83">
         <v>1373</v>
@@ -3369,7 +3313,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -3389,7 +3333,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -3400,16 +3344,16 @@
         <v>175</v>
       </c>
       <c r="D85">
-        <v>9201</v>
+        <v>9202</v>
       </c>
       <c r="E85">
-        <v>4058</v>
+        <v>4059</v>
       </c>
       <c r="F85" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -3420,16 +3364,16 @@
         <v>176</v>
       </c>
       <c r="D86">
-        <v>112493</v>
+        <v>112527</v>
       </c>
       <c r="E86">
-        <v>45313</v>
+        <v>45329</v>
       </c>
       <c r="F86" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -3440,16 +3384,16 @@
         <v>177</v>
       </c>
       <c r="D87">
-        <v>304702</v>
+        <v>304743</v>
       </c>
       <c r="E87">
-        <v>94985</v>
+        <v>94996</v>
       </c>
       <c r="F87" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -3460,16 +3404,16 @@
         <v>178</v>
       </c>
       <c r="D88">
-        <v>467152</v>
+        <v>467329</v>
       </c>
       <c r="E88">
-        <v>145631</v>
+        <v>145669</v>
       </c>
       <c r="F88" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -3480,16 +3424,16 @@
         <v>179</v>
       </c>
       <c r="D89">
-        <v>90295</v>
+        <v>90309</v>
       </c>
       <c r="E89">
-        <v>33007</v>
+        <v>33010</v>
       </c>
       <c r="F89" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -3509,7 +3453,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -3529,7 +3473,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -3549,7 +3493,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -3560,7 +3504,7 @@
         <v>183</v>
       </c>
       <c r="D93">
-        <v>9637</v>
+        <v>9638</v>
       </c>
       <c r="E93">
         <v>2511</v>
@@ -3569,7 +3513,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -3589,7 +3533,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -3600,16 +3544,16 @@
         <v>185</v>
       </c>
       <c r="D95">
-        <v>39219</v>
+        <v>39247</v>
       </c>
       <c r="E95">
-        <v>13515</v>
+        <v>13521</v>
       </c>
       <c r="F95" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -3620,16 +3564,16 @@
         <v>186</v>
       </c>
       <c r="D96">
-        <v>6337</v>
+        <v>6339</v>
       </c>
       <c r="E96">
-        <v>2167</v>
+        <v>2168</v>
       </c>
       <c r="F96" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -3640,16 +3584,16 @@
         <v>187</v>
       </c>
       <c r="D97">
-        <v>51983</v>
+        <v>52038</v>
       </c>
       <c r="E97">
-        <v>14413</v>
+        <v>14428</v>
       </c>
       <c r="F97" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -3660,16 +3604,16 @@
         <v>188</v>
       </c>
       <c r="D98">
-        <v>77806</v>
+        <v>77842</v>
       </c>
       <c r="E98">
-        <v>28233</v>
+        <v>28247</v>
       </c>
       <c r="F98" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -3680,16 +3624,16 @@
         <v>189</v>
       </c>
       <c r="D99">
-        <v>5799</v>
+        <v>5800</v>
       </c>
       <c r="E99">
-        <v>2916</v>
+        <v>2917</v>
       </c>
       <c r="F99" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -3700,16 +3644,16 @@
         <v>190</v>
       </c>
       <c r="D100">
-        <v>14721</v>
+        <v>14725</v>
       </c>
       <c r="E100">
-        <v>4465</v>
+        <v>4467</v>
       </c>
       <c r="F100" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -3720,10 +3664,10 @@
         <v>191</v>
       </c>
       <c r="D101">
-        <v>11996</v>
+        <v>12006</v>
       </c>
       <c r="E101">
-        <v>4170</v>
+        <v>4174</v>
       </c>
       <c r="F101" t="s">
         <v>251</v>
@@ -3735,16 +3679,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3761,7 +3703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3772,16 +3714,16 @@
         <v>312</v>
       </c>
       <c r="D2">
-        <v>4109033</v>
+        <v>4109365</v>
       </c>
       <c r="E2">
-        <v>696804</v>
+        <v>696850</v>
       </c>
       <c r="F2" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3792,16 +3734,16 @@
         <v>313</v>
       </c>
       <c r="D3">
-        <v>3400878</v>
+        <v>3401013</v>
       </c>
       <c r="E3">
-        <v>598992</v>
+        <v>599010</v>
       </c>
       <c r="F3" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3812,16 +3754,16 @@
         <v>314</v>
       </c>
       <c r="D4">
-        <v>160190</v>
+        <v>160288</v>
       </c>
       <c r="E4">
-        <v>46206</v>
+        <v>46237</v>
       </c>
       <c r="F4" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3832,16 +3774,16 @@
         <v>315</v>
       </c>
       <c r="D5">
-        <v>1458674</v>
+        <v>1459708</v>
       </c>
       <c r="E5">
-        <v>363827</v>
+        <v>364031</v>
       </c>
       <c r="F5" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3852,16 +3794,16 @@
         <v>316</v>
       </c>
       <c r="D6">
-        <v>1805568</v>
+        <v>1805782</v>
       </c>
       <c r="E6">
-        <v>400366</v>
+        <v>400416</v>
       </c>
       <c r="F6" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3872,16 +3814,16 @@
         <v>317</v>
       </c>
       <c r="D7">
-        <v>499334</v>
+        <v>499767</v>
       </c>
       <c r="E7">
-        <v>154352</v>
+        <v>154442</v>
       </c>
       <c r="F7" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3892,16 +3834,16 @@
         <v>318</v>
       </c>
       <c r="D8">
-        <v>772949</v>
+        <v>773267</v>
       </c>
       <c r="E8">
-        <v>247526</v>
+        <v>247613</v>
       </c>
       <c r="F8" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3912,16 +3854,16 @@
         <v>319</v>
       </c>
       <c r="D9">
-        <v>27642</v>
+        <v>27692</v>
       </c>
       <c r="E9">
-        <v>8188</v>
+        <v>8196</v>
       </c>
       <c r="F9" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3932,16 +3874,16 @@
         <v>320</v>
       </c>
       <c r="D10">
-        <v>67699</v>
+        <v>67721</v>
       </c>
       <c r="E10">
-        <v>13997</v>
+        <v>14003</v>
       </c>
       <c r="F10" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3952,16 +3894,16 @@
         <v>321</v>
       </c>
       <c r="D11">
-        <v>740759</v>
+        <v>741198</v>
       </c>
       <c r="E11">
-        <v>206332</v>
+        <v>206424</v>
       </c>
       <c r="F11" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3972,16 +3914,16 @@
         <v>322</v>
       </c>
       <c r="D12">
-        <v>130482</v>
+        <v>130516</v>
       </c>
       <c r="E12">
-        <v>39084</v>
+        <v>39089</v>
       </c>
       <c r="F12" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3992,16 +3934,16 @@
         <v>323</v>
       </c>
       <c r="D13">
-        <v>50076</v>
+        <v>50135</v>
       </c>
       <c r="E13">
-        <v>16098</v>
+        <v>16116</v>
       </c>
       <c r="F13" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -4012,16 +3954,16 @@
         <v>324</v>
       </c>
       <c r="D14">
-        <v>3938797</v>
+        <v>3939016</v>
       </c>
       <c r="E14">
-        <v>672781</v>
+        <v>672797</v>
       </c>
       <c r="F14" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -4032,16 +3974,16 @@
         <v>325</v>
       </c>
       <c r="D15">
-        <v>4026135</v>
+        <v>4026316</v>
       </c>
       <c r="E15">
-        <v>703392</v>
+        <v>703418</v>
       </c>
       <c r="F15" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -4052,16 +3994,16 @@
         <v>326</v>
       </c>
       <c r="D16">
-        <v>507456</v>
+        <v>507747</v>
       </c>
       <c r="E16">
-        <v>152112</v>
+        <v>152167</v>
       </c>
       <c r="F16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -4072,16 +4014,16 @@
         <v>327</v>
       </c>
       <c r="D17">
-        <v>1823418</v>
+        <v>1823523</v>
       </c>
       <c r="E17">
-        <v>357271</v>
+        <v>357287</v>
       </c>
       <c r="F17" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -4092,16 +4034,16 @@
         <v>328</v>
       </c>
       <c r="D18">
-        <v>84139</v>
+        <v>84146</v>
       </c>
       <c r="E18">
-        <v>28393</v>
+        <v>28395</v>
       </c>
       <c r="F18" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -4121,7 +4063,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -4141,7 +4083,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -4152,16 +4094,16 @@
         <v>331</v>
       </c>
       <c r="D21">
-        <v>677201</v>
+        <v>677670</v>
       </c>
       <c r="E21">
-        <v>191025</v>
+        <v>191105</v>
       </c>
       <c r="F21" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -4172,16 +4114,16 @@
         <v>332</v>
       </c>
       <c r="D22">
-        <v>353681</v>
+        <v>353842</v>
       </c>
       <c r="E22">
-        <v>112087</v>
+        <v>112147</v>
       </c>
       <c r="F22" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -4192,16 +4134,16 @@
         <v>333</v>
       </c>
       <c r="D23">
-        <v>46166</v>
+        <v>46197</v>
       </c>
       <c r="E23">
-        <v>13692</v>
+        <v>13696</v>
       </c>
       <c r="F23" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -4212,16 +4154,16 @@
         <v>334</v>
       </c>
       <c r="D24">
-        <v>90061</v>
+        <v>90083</v>
       </c>
       <c r="E24">
-        <v>21119</v>
+        <v>21122</v>
       </c>
       <c r="F24" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -4232,16 +4174,16 @@
         <v>335</v>
       </c>
       <c r="D25">
-        <v>31645</v>
+        <v>31652</v>
       </c>
       <c r="E25">
-        <v>10445</v>
+        <v>10446</v>
       </c>
       <c r="F25" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -4252,16 +4194,16 @@
         <v>336</v>
       </c>
       <c r="D26">
-        <v>9480</v>
+        <v>9484</v>
       </c>
       <c r="E26">
-        <v>2526</v>
+        <v>2528</v>
       </c>
       <c r="F26" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -4272,16 +4214,16 @@
         <v>337</v>
       </c>
       <c r="D27">
-        <v>52656</v>
+        <v>52679</v>
       </c>
       <c r="E27">
-        <v>16128</v>
+        <v>16133</v>
       </c>
       <c r="F27" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -4292,16 +4234,16 @@
         <v>338</v>
       </c>
       <c r="D28">
-        <v>40124</v>
+        <v>40138</v>
       </c>
       <c r="E28">
-        <v>12558</v>
+        <v>12564</v>
       </c>
       <c r="F28" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -4312,16 +4254,16 @@
         <v>339</v>
       </c>
       <c r="D29">
-        <v>76925</v>
+        <v>76949</v>
       </c>
       <c r="E29">
-        <v>31747</v>
+        <v>31755</v>
       </c>
       <c r="F29" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -4332,16 +4274,16 @@
         <v>340</v>
       </c>
       <c r="D30">
-        <v>409163</v>
+        <v>409854</v>
       </c>
       <c r="E30">
-        <v>96198</v>
+        <v>96353</v>
       </c>
       <c r="F30" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -4352,16 +4294,16 @@
         <v>341</v>
       </c>
       <c r="D31">
-        <v>176719</v>
+        <v>176762</v>
       </c>
       <c r="E31">
-        <v>55232</v>
+        <v>55243</v>
       </c>
       <c r="F31" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -4372,16 +4314,16 @@
         <v>342</v>
       </c>
       <c r="D32">
-        <v>122246</v>
+        <v>122288</v>
       </c>
       <c r="E32">
-        <v>33521</v>
+        <v>33528</v>
       </c>
       <c r="F32" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -4392,7 +4334,7 @@
         <v>343</v>
       </c>
       <c r="D33">
-        <v>7174</v>
+        <v>7175</v>
       </c>
       <c r="E33">
         <v>2449</v>
@@ -4401,7 +4343,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -4412,16 +4354,16 @@
         <v>344</v>
       </c>
       <c r="D34">
-        <v>988475</v>
+        <v>989074</v>
       </c>
       <c r="E34">
-        <v>282582</v>
+        <v>282739</v>
       </c>
       <c r="F34" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -4441,7 +4383,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -4452,16 +4394,16 @@
         <v>346</v>
       </c>
       <c r="D36">
-        <v>185294</v>
+        <v>185355</v>
       </c>
       <c r="E36">
-        <v>48993</v>
+        <v>49012</v>
       </c>
       <c r="F36" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -4472,16 +4414,16 @@
         <v>347</v>
       </c>
       <c r="D37">
-        <v>430561</v>
+        <v>431052</v>
       </c>
       <c r="E37">
-        <v>94045</v>
+        <v>94139</v>
       </c>
       <c r="F37" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -4492,16 +4434,16 @@
         <v>348</v>
       </c>
       <c r="D38">
-        <v>739787</v>
+        <v>740142</v>
       </c>
       <c r="E38">
-        <v>209119</v>
+        <v>209205</v>
       </c>
       <c r="F38" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -4512,16 +4454,16 @@
         <v>349</v>
       </c>
       <c r="D39">
-        <v>5754729</v>
+        <v>5757895</v>
       </c>
       <c r="E39">
-        <v>1003264</v>
+        <v>1003651</v>
       </c>
       <c r="F39" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -4532,16 +4474,16 @@
         <v>350</v>
       </c>
       <c r="D40">
-        <v>20711</v>
+        <v>20720</v>
       </c>
       <c r="E40">
-        <v>6995</v>
+        <v>6999</v>
       </c>
       <c r="F40" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -4552,16 +4494,16 @@
         <v>351</v>
       </c>
       <c r="D41">
-        <v>3227496</v>
+        <v>3227729</v>
       </c>
       <c r="E41">
-        <v>498807</v>
+        <v>498851</v>
       </c>
       <c r="F41" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -4572,16 +4514,16 @@
         <v>139</v>
       </c>
       <c r="D42">
-        <v>57965</v>
+        <v>57971</v>
       </c>
       <c r="E42">
-        <v>23650</v>
+        <v>23651</v>
       </c>
       <c r="F42" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -4592,16 +4534,16 @@
         <v>352</v>
       </c>
       <c r="D43">
-        <v>5844</v>
+        <v>5848</v>
       </c>
       <c r="E43">
-        <v>2305</v>
+        <v>2308</v>
       </c>
       <c r="F43" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -4612,16 +4554,16 @@
         <v>353</v>
       </c>
       <c r="D44">
-        <v>21593</v>
+        <v>21605</v>
       </c>
       <c r="E44">
-        <v>7501</v>
+        <v>7505</v>
       </c>
       <c r="F44" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -4632,16 +4574,16 @@
         <v>354</v>
       </c>
       <c r="D45">
-        <v>123508</v>
+        <v>123540</v>
       </c>
       <c r="E45">
-        <v>40127</v>
+        <v>40140</v>
       </c>
       <c r="F45" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -4652,16 +4594,16 @@
         <v>355</v>
       </c>
       <c r="D46">
-        <v>38585</v>
+        <v>38596</v>
       </c>
       <c r="E46">
-        <v>10307</v>
+        <v>10312</v>
       </c>
       <c r="F46" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -4672,16 +4614,16 @@
         <v>356</v>
       </c>
       <c r="D47">
-        <v>113600</v>
+        <v>113681</v>
       </c>
       <c r="E47">
-        <v>27549</v>
+        <v>27599</v>
       </c>
       <c r="F47" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -4692,7 +4634,7 @@
         <v>357</v>
       </c>
       <c r="D48">
-        <v>80554</v>
+        <v>80565</v>
       </c>
       <c r="E48">
         <v>34614</v>
@@ -4701,7 +4643,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -4712,16 +4654,16 @@
         <v>358</v>
       </c>
       <c r="D49">
-        <v>24984</v>
+        <v>24988</v>
       </c>
       <c r="E49">
-        <v>10343</v>
+        <v>10345</v>
       </c>
       <c r="F49" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -4732,16 +4674,16 @@
         <v>359</v>
       </c>
       <c r="D50">
-        <v>108256</v>
+        <v>108281</v>
       </c>
       <c r="E50">
-        <v>36099</v>
+        <v>36105</v>
       </c>
       <c r="F50" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -4752,16 +4694,16 @@
         <v>360</v>
       </c>
       <c r="D51">
-        <v>324973</v>
+        <v>325073</v>
       </c>
       <c r="E51">
-        <v>88331</v>
+        <v>88354</v>
       </c>
       <c r="F51" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -4781,7 +4723,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -4792,16 +4734,16 @@
         <v>362</v>
       </c>
       <c r="D53">
-        <v>4105919</v>
+        <v>4106123</v>
       </c>
       <c r="E53">
-        <v>694645</v>
+        <v>694667</v>
       </c>
       <c r="F53" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -4812,16 +4754,16 @@
         <v>363</v>
       </c>
       <c r="D54">
-        <v>111565</v>
+        <v>111578</v>
       </c>
       <c r="E54">
-        <v>32584</v>
+        <v>32590</v>
       </c>
       <c r="F54" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -4832,16 +4774,16 @@
         <v>364</v>
       </c>
       <c r="D55">
-        <v>14757</v>
+        <v>14764</v>
       </c>
       <c r="E55">
-        <v>6220</v>
+        <v>6222</v>
       </c>
       <c r="F55" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -4852,16 +4794,16 @@
         <v>365</v>
       </c>
       <c r="D56">
-        <v>1285000</v>
+        <v>1285093</v>
       </c>
       <c r="E56">
-        <v>245237</v>
+        <v>245258</v>
       </c>
       <c r="F56" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -4872,16 +4814,16 @@
         <v>366</v>
       </c>
       <c r="D57">
-        <v>71173</v>
+        <v>71190</v>
       </c>
       <c r="E57">
-        <v>32366</v>
+        <v>32376</v>
       </c>
       <c r="F57" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -4892,16 +4834,16 @@
         <v>367</v>
       </c>
       <c r="D58">
-        <v>540708</v>
+        <v>540944</v>
       </c>
       <c r="E58">
-        <v>172723</v>
+        <v>172787</v>
       </c>
       <c r="F58" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -4912,16 +4854,16 @@
         <v>368</v>
       </c>
       <c r="D59">
-        <v>17343</v>
+        <v>17350</v>
       </c>
       <c r="E59">
-        <v>4607</v>
+        <v>4609</v>
       </c>
       <c r="F59" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -4932,16 +4874,16 @@
         <v>369</v>
       </c>
       <c r="D60">
-        <v>28513</v>
+        <v>28520</v>
       </c>
       <c r="E60">
-        <v>11985</v>
+        <v>11989</v>
       </c>
       <c r="F60" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -4952,16 +4894,16 @@
         <v>370</v>
       </c>
       <c r="D61">
-        <v>296937</v>
+        <v>297038</v>
       </c>
       <c r="E61">
-        <v>97065</v>
+        <v>97086</v>
       </c>
       <c r="F61" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -4972,16 +4914,16 @@
         <v>371</v>
       </c>
       <c r="D62">
-        <v>16977</v>
+        <v>16987</v>
       </c>
       <c r="E62">
-        <v>5995</v>
+        <v>5996</v>
       </c>
       <c r="F62" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -4992,16 +4934,16 @@
         <v>372</v>
       </c>
       <c r="D63">
-        <v>67185</v>
+        <v>67242</v>
       </c>
       <c r="E63">
-        <v>24064</v>
+        <v>24083</v>
       </c>
       <c r="F63" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -5012,16 +4954,16 @@
         <v>373</v>
       </c>
       <c r="D64">
-        <v>11906</v>
+        <v>11909</v>
       </c>
       <c r="E64">
-        <v>3530</v>
+        <v>3531</v>
       </c>
       <c r="F64" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -5032,7 +4974,7 @@
         <v>374</v>
       </c>
       <c r="D65">
-        <v>57670</v>
+        <v>57681</v>
       </c>
       <c r="E65">
         <v>12395</v>
@@ -5041,7 +4983,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -5061,7 +5003,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -5081,7 +5023,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -5092,16 +5034,16 @@
         <v>377</v>
       </c>
       <c r="D68">
-        <v>9795</v>
+        <v>9799</v>
       </c>
       <c r="E68">
-        <v>2845</v>
+        <v>2847</v>
       </c>
       <c r="F68" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -5112,16 +5054,16 @@
         <v>378</v>
       </c>
       <c r="D69">
-        <v>20032</v>
+        <v>20033</v>
       </c>
       <c r="E69">
-        <v>6088</v>
+        <v>6089</v>
       </c>
       <c r="F69" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -5132,16 +5074,16 @@
         <v>379</v>
       </c>
       <c r="D70">
-        <v>539692</v>
+        <v>539865</v>
       </c>
       <c r="E70">
-        <v>160206</v>
+        <v>160249</v>
       </c>
       <c r="F70" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -5161,7 +5103,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -5172,16 +5114,16 @@
         <v>381</v>
       </c>
       <c r="D72">
-        <v>553218</v>
+        <v>553458</v>
       </c>
       <c r="E72">
-        <v>179544</v>
+        <v>179622</v>
       </c>
       <c r="F72" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -5192,16 +5134,16 @@
         <v>382</v>
       </c>
       <c r="D73">
-        <v>174952</v>
+        <v>174980</v>
       </c>
       <c r="E73">
-        <v>55492</v>
+        <v>55502</v>
       </c>
       <c r="F73" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -5221,7 +5163,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -5232,16 +5174,16 @@
         <v>384</v>
       </c>
       <c r="D75">
-        <v>244588</v>
+        <v>244683</v>
       </c>
       <c r="E75">
-        <v>80350</v>
+        <v>80379</v>
       </c>
       <c r="F75" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -5261,7 +5203,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -5272,16 +5214,16 @@
         <v>386</v>
       </c>
       <c r="D77">
-        <v>1000998</v>
+        <v>1001243</v>
       </c>
       <c r="E77">
-        <v>211401</v>
+        <v>211458</v>
       </c>
       <c r="F77" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -5292,16 +5234,16 @@
         <v>387</v>
       </c>
       <c r="D78">
-        <v>14332</v>
+        <v>14335</v>
       </c>
       <c r="E78">
-        <v>5663</v>
+        <v>5665</v>
       </c>
       <c r="F78" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -5312,16 +5254,16 @@
         <v>388</v>
       </c>
       <c r="D79">
-        <v>27403</v>
+        <v>27411</v>
       </c>
       <c r="E79">
-        <v>11451</v>
+        <v>11454</v>
       </c>
       <c r="F79" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -5332,16 +5274,16 @@
         <v>389</v>
       </c>
       <c r="D80">
-        <v>3112044</v>
+        <v>3112257</v>
       </c>
       <c r="E80">
-        <v>698021</v>
+        <v>698045</v>
       </c>
       <c r="F80" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -5352,7 +5294,7 @@
         <v>390</v>
       </c>
       <c r="D81">
-        <v>12749</v>
+        <v>12750</v>
       </c>
       <c r="E81">
         <v>6578</v>
@@ -5361,7 +5303,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -5372,16 +5314,16 @@
         <v>391</v>
       </c>
       <c r="D82">
-        <v>58563</v>
+        <v>58588</v>
       </c>
       <c r="E82">
-        <v>27824</v>
+        <v>27829</v>
       </c>
       <c r="F82" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -5392,7 +5334,7 @@
         <v>392</v>
       </c>
       <c r="D83">
-        <v>18140</v>
+        <v>18145</v>
       </c>
       <c r="E83">
         <v>6049</v>
@@ -5401,7 +5343,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -5412,16 +5354,16 @@
         <v>393</v>
       </c>
       <c r="D84">
-        <v>85812</v>
+        <v>85866</v>
       </c>
       <c r="E84">
-        <v>29160</v>
+        <v>29173</v>
       </c>
       <c r="F84" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -5432,7 +5374,7 @@
         <v>394</v>
       </c>
       <c r="D85">
-        <v>10379</v>
+        <v>10381</v>
       </c>
       <c r="E85">
         <v>3835</v>
@@ -5441,7 +5383,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -5452,16 +5394,16 @@
         <v>395</v>
       </c>
       <c r="D86">
-        <v>37301</v>
+        <v>37475</v>
       </c>
       <c r="E86">
-        <v>12867</v>
+        <v>12898</v>
       </c>
       <c r="F86" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -5472,16 +5414,16 @@
         <v>396</v>
       </c>
       <c r="D87">
-        <v>23944</v>
+        <v>23964</v>
       </c>
       <c r="E87">
-        <v>10069</v>
+        <v>10079</v>
       </c>
       <c r="F87" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -5492,16 +5434,16 @@
         <v>397</v>
       </c>
       <c r="D88">
-        <v>94592</v>
+        <v>94596</v>
       </c>
       <c r="E88">
-        <v>35998</v>
+        <v>36000</v>
       </c>
       <c r="F88" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -5521,7 +5463,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -5532,16 +5474,16 @@
         <v>399</v>
       </c>
       <c r="D90">
-        <v>74045</v>
+        <v>74050</v>
       </c>
       <c r="E90">
-        <v>28652</v>
+        <v>28653</v>
       </c>
       <c r="F90" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -5561,7 +5503,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -5572,16 +5514,16 @@
         <v>401</v>
       </c>
       <c r="D92">
-        <v>31945</v>
+        <v>31946</v>
       </c>
       <c r="E92">
-        <v>9237</v>
+        <v>9238</v>
       </c>
       <c r="F92" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -5592,16 +5534,16 @@
         <v>402</v>
       </c>
       <c r="D93">
-        <v>37282</v>
+        <v>37296</v>
       </c>
       <c r="E93">
-        <v>11119</v>
+        <v>11123</v>
       </c>
       <c r="F93" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -5612,7 +5554,7 @@
         <v>403</v>
       </c>
       <c r="D94">
-        <v>13221</v>
+        <v>13223</v>
       </c>
       <c r="E94">
         <v>5300</v>
@@ -5621,7 +5563,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -5632,16 +5574,16 @@
         <v>404</v>
       </c>
       <c r="D95">
-        <v>29962</v>
+        <v>29971</v>
       </c>
       <c r="E95">
-        <v>10565</v>
+        <v>10566</v>
       </c>
       <c r="F95" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -5652,16 +5594,16 @@
         <v>405</v>
       </c>
       <c r="D96">
-        <v>2527491</v>
+        <v>2527641</v>
       </c>
       <c r="E96">
-        <v>420307</v>
+        <v>420321</v>
       </c>
       <c r="F96" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -5681,7 +5623,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -5701,7 +5643,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -5712,16 +5654,16 @@
         <v>408</v>
       </c>
       <c r="D99">
-        <v>14070</v>
+        <v>14075</v>
       </c>
       <c r="E99">
-        <v>4951</v>
+        <v>4954</v>
       </c>
       <c r="F99" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -5732,16 +5674,16 @@
         <v>409</v>
       </c>
       <c r="D100">
-        <v>1030090</v>
+        <v>1030621</v>
       </c>
       <c r="E100">
-        <v>287487</v>
+        <v>287586</v>
       </c>
       <c r="F100" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -5752,10 +5694,10 @@
         <v>410</v>
       </c>
       <c r="D101">
-        <v>296355</v>
+        <v>296391</v>
       </c>
       <c r="E101">
-        <v>87829</v>
+        <v>87838</v>
       </c>
       <c r="F101" t="s">
         <v>248</v>

</xml_diff>